<commit_message>
indicate cover is alternate
</commit_message>
<xml_diff>
--- a/metalhead/checklist.xlsx
+++ b/metalhead/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Source/japanese-collectors-list/metalhead/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C903F5C-A76F-4D4A-A0EC-8DCDE3BCF29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C040DDCD-FDDA-7249-B001-3C3D9F16C0E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="25480" windowHeight="16340" xr2:uid="{AA506737-A005-B24A-B9DB-FD3A738B7EAA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="69">
   <si>
     <t>year</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>metalhead_alternate.jpg</t>
+  </si>
+  <si>
+    <t>Metal Head (alternate cover)</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,7 +668,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>

</xml_diff>